<commit_message>
1-2, 1-3, 1-4 recommit
Success/failure judgment
</commit_message>
<xml_diff>
--- a/Assets/ExcelFile/1_PoliceNote.csv.xlsx
+++ b/Assets/ExcelFile/1_PoliceNote.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityProject\test\Poliverse-Fork\Assets\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427BC7F9-B37E-463E-933A-EF678B56C606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB86D09-C1F5-4DC4-91BC-90C6976E45B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{F8F1257B-76BA-4C6F-AD5C-8DA409C9F897}"/>
   </bookViews>
@@ -487,7 +487,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -542,7 +542,7 @@
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
-        <f t="shared" ref="A4" si="0">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f>"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-2_time</v>
       </c>
       <c r="B4" s="5">
@@ -551,7 +551,7 @@
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
-        <f t="shared" ref="A5" si="1">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A5" si="0">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-2_type</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -560,7 +560,7 @@
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
-        <f t="shared" ref="A6" si="2">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f t="shared" ref="A6" si="1">"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-3_time</v>
       </c>
       <c r="B6" s="5">
@@ -578,7 +578,7 @@
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
-        <f t="shared" ref="A7" si="3">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A7" si="2">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-3_type</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -596,7 +596,7 @@
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
-        <f t="shared" ref="A8" si="4">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f t="shared" ref="A8" si="3">"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-4_time</v>
       </c>
       <c r="B8" s="5">
@@ -614,7 +614,7 @@
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
-        <f t="shared" ref="A9" si="5">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A9" si="4">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-4_type</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -632,7 +632,7 @@
     </row>
     <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
-        <f t="shared" ref="A10" si="6">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f t="shared" ref="A10" si="5">"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-5_time</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -650,7 +650,7 @@
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
-        <f t="shared" ref="A11" si="7">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A11" si="6">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-5_type</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -668,7 +668,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
-        <f t="shared" ref="A12" si="8">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f t="shared" ref="A12" si="7">"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-6_time</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -686,7 +686,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
-        <f t="shared" ref="A13" si="9">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A13" si="8">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-6_type</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -704,7 +704,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
-        <f t="shared" ref="A14" si="10">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f t="shared" ref="A14" si="9">"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-7_time</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -722,7 +722,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
-        <f t="shared" ref="A15" si="11">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A15" si="10">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-7_type</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -740,7 +740,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
-        <f t="shared" ref="A16" si="12">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f t="shared" ref="A16" si="11">"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-8_time</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -758,7 +758,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
-        <f t="shared" ref="A17" si="13">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A17" si="12">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-8_type</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -776,7 +776,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
-        <f t="shared" ref="A18" si="14">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f t="shared" ref="A18" si="13">"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-9_time</v>
       </c>
       <c r="B18" s="5">
@@ -794,7 +794,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
-        <f t="shared" ref="A19" si="15">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A19" si="14">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-9_type</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -812,7 +812,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
-        <f t="shared" ref="A20" si="16">"1-" &amp; ROW()/2 &amp; "_time"</f>
+        <f t="shared" ref="A20" si="15">"1-" &amp; ROW()/2 &amp; "_time"</f>
         <v>1-10_time</v>
       </c>
       <c r="B20" s="5">
@@ -830,7 +830,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
-        <f t="shared" ref="A21" si="17">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
+        <f t="shared" ref="A21" si="16">"1-" &amp; (ROW()-1)/2 &amp; "_type"</f>
         <v>1-10_type</v>
       </c>
       <c r="B21" s="4" t="s">

</xml_diff>